<commit_message>
Iteration 14 branch compilation issues fixes
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation/TestData/TestData.xlsx
+++ b/src/main/resources/config/automation/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15108" windowHeight="8988" firstSheet="11" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15672" windowHeight="8976" firstSheet="14" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="S181372" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,15 @@
     <sheet name="CurrencyExchangeRateUpload" sheetId="13" r:id="rId13"/>
     <sheet name="CurrencyExchangeRateMapping" sheetId="14" r:id="rId14"/>
     <sheet name="LoyaltyPlan" sheetId="16" r:id="rId15"/>
+    <sheet name="Prepaid_Application_Upload" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:E21"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1600" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1846" uniqueCount="539">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1642,6 +1644,9 @@
   </si>
   <si>
     <t>121212</t>
+  </si>
+  <si>
+    <t>TC_Application_Upload_Prepaid</t>
   </si>
 </sst>
 </file>
@@ -3686,8 +3691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DL1" workbookViewId="0">
-      <selection activeCell="EB6" sqref="EB6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4484,6 +4489,811 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:EE2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:135" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AM1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AN1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AO1" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="AP1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AQ1" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AR1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS1" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AT1" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BE1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="BH1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="BI1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="BJ1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="BK1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="BL1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="BM1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="BN1" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="BO1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="BP1" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="BQ1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BR1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="BS1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="BT1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="BU1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="BV1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="BW1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="BX1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BY1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="BZ1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="CA1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="CB1" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="CC1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="CD1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="CE1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="CF1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="CG1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="CH1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="CI1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="CJ1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="CK1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="CL1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="CM1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="CN1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="CO1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="CP1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="CQ1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="CR1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="CS1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="CT1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="CU1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="CV1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="CW1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="CX1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="CY1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="CZ1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="DA1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="DB1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="DC1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="DD1" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="DE1" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="DF1" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="DG1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="DH1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="DI1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="DJ1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="DK1" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="DL1" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="DM1" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="DN1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="DO1" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="DP1" s="38" t="s">
+        <v>475</v>
+      </c>
+      <c r="DQ1" s="38" t="s">
+        <v>476</v>
+      </c>
+      <c r="DR1" s="38" t="s">
+        <v>477</v>
+      </c>
+      <c r="DS1" s="38" t="s">
+        <v>478</v>
+      </c>
+      <c r="DT1" s="38" t="s">
+        <v>479</v>
+      </c>
+      <c r="DU1" s="38" t="s">
+        <v>480</v>
+      </c>
+      <c r="DV1" s="38" t="s">
+        <v>481</v>
+      </c>
+      <c r="DW1" s="38" t="s">
+        <v>482</v>
+      </c>
+      <c r="DX1" s="38" t="s">
+        <v>483</v>
+      </c>
+      <c r="DY1" s="38" t="s">
+        <v>484</v>
+      </c>
+      <c r="DZ1" s="38" t="s">
+        <v>485</v>
+      </c>
+      <c r="EA1" s="38" t="s">
+        <v>486</v>
+      </c>
+      <c r="EB1" s="38" t="s">
+        <v>487</v>
+      </c>
+      <c r="EC1" s="38" t="s">
+        <v>488</v>
+      </c>
+      <c r="ED1" s="38" t="s">
+        <v>489</v>
+      </c>
+      <c r="EE1" s="38" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="2" spans="1:135" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="B2" t="s">
+        <v>531</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>537</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>494</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="K2" s="39" t="s">
+        <v>496</v>
+      </c>
+      <c r="L2" s="39" t="s">
+        <v>497</v>
+      </c>
+      <c r="M2" s="39" t="s">
+        <v>498</v>
+      </c>
+      <c r="N2" s="40" t="s">
+        <v>499</v>
+      </c>
+      <c r="O2" s="40" t="s">
+        <v>500</v>
+      </c>
+      <c r="P2" s="40" t="s">
+        <v>500</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="R2" s="40" t="s">
+        <v>502</v>
+      </c>
+      <c r="S2" s="40" t="s">
+        <v>533</v>
+      </c>
+      <c r="T2" s="40" t="s">
+        <v>503</v>
+      </c>
+      <c r="U2" s="11">
+        <v>50</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="X2" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z2" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA2" s="42"/>
+      <c r="AB2" s="42"/>
+      <c r="AC2" s="12"/>
+      <c r="AD2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE2" s="12"/>
+      <c r="AF2" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="AG2" s="12" t="s">
+        <v>505</v>
+      </c>
+      <c r="AH2" s="12" t="s">
+        <v>506</v>
+      </c>
+      <c r="AI2" s="12" t="s">
+        <v>507</v>
+      </c>
+      <c r="AJ2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK2" s="12">
+        <v>1989</v>
+      </c>
+      <c r="AL2" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM2" s="14">
+        <v>12345678</v>
+      </c>
+      <c r="AN2" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="AO2" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP2" s="12" t="s">
+        <v>508</v>
+      </c>
+      <c r="AQ2" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AR2" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="AS2" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="AT2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU2" s="11"/>
+      <c r="AV2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AW2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="AX2" s="11">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AZ2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="BA2" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB2" s="12">
+        <v>1</v>
+      </c>
+      <c r="BC2" s="12" t="s">
+        <v>509</v>
+      </c>
+      <c r="BD2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="BE2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="BF2" s="12">
+        <v>12</v>
+      </c>
+      <c r="BG2" s="12" t="s">
+        <v>510</v>
+      </c>
+      <c r="BH2" s="12">
+        <v>2</v>
+      </c>
+      <c r="BI2" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="BJ2" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="BK2" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="BL2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="BM2" s="12" t="s">
+        <v>511</v>
+      </c>
+      <c r="BN2" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="BO2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="BP2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="BQ2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="BR2" s="41" t="s">
+        <v>416</v>
+      </c>
+      <c r="BS2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="BT2" s="12">
+        <v>12345678</v>
+      </c>
+      <c r="BU2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="BV2" s="12">
+        <v>12345678</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>512</v>
+      </c>
+      <c r="BX2" s="45"/>
+      <c r="BY2" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="BZ2" s="12" t="s">
+        <v>510</v>
+      </c>
+      <c r="CA2" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="CB2" s="12" t="s">
+        <v>513</v>
+      </c>
+      <c r="CC2" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="CD2" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="CE2" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="CF2" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="CG2" s="12"/>
+      <c r="CH2" s="45" t="s">
+        <v>415</v>
+      </c>
+      <c r="CI2" s="45" t="s">
+        <v>417</v>
+      </c>
+      <c r="CJ2" s="42"/>
+      <c r="CK2" s="42"/>
+      <c r="CL2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="CM2" s="45" t="s">
+        <v>530</v>
+      </c>
+      <c r="CN2" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="CO2" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="CP2" s="42" t="s">
+        <v>356</v>
+      </c>
+      <c r="CQ2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="CR2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="CS2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="CT2" s="11"/>
+      <c r="CU2" s="11"/>
+      <c r="CV2" s="42" t="s">
+        <v>500</v>
+      </c>
+      <c r="CW2" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="CX2" s="42" t="s">
+        <v>419</v>
+      </c>
+      <c r="CY2" s="42" t="s">
+        <v>415</v>
+      </c>
+      <c r="CZ2" s="42" t="s">
+        <v>420</v>
+      </c>
+      <c r="DA2" s="42" t="s">
+        <v>421</v>
+      </c>
+      <c r="DB2" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="DC2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="DD2" s="12"/>
+      <c r="DE2" s="12"/>
+      <c r="DF2" s="12"/>
+      <c r="DG2" s="12"/>
+      <c r="DH2" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="DI2" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="DJ2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="DK2" s="11" t="s">
+        <v>514</v>
+      </c>
+      <c r="DL2" s="11" t="s">
+        <v>515</v>
+      </c>
+      <c r="DM2" s="12" t="s">
+        <v>516</v>
+      </c>
+      <c r="DN2" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="DO2" s="11" t="s">
+        <v>517</v>
+      </c>
+      <c r="DP2" s="43" t="s">
+        <v>518</v>
+      </c>
+      <c r="DQ2" s="43" t="s">
+        <v>519</v>
+      </c>
+      <c r="DR2" s="43" t="s">
+        <v>520</v>
+      </c>
+      <c r="DS2" s="44" t="s">
+        <v>521</v>
+      </c>
+      <c r="DT2" s="44" t="s">
+        <v>415</v>
+      </c>
+      <c r="DU2" s="44" t="s">
+        <v>522</v>
+      </c>
+      <c r="DV2" s="43" t="s">
+        <v>523</v>
+      </c>
+      <c r="DW2" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="DX2" s="44" t="s">
+        <v>414</v>
+      </c>
+      <c r="DY2" s="44" t="s">
+        <v>524</v>
+      </c>
+      <c r="DZ2" s="44" t="s">
+        <v>525</v>
+      </c>
+      <c r="EA2" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="EB2" s="44" t="s">
+        <v>525</v>
+      </c>
+      <c r="EC2" s="44" t="s">
+        <v>526</v>
+      </c>
+      <c r="ED2" s="44" t="s">
+        <v>527</v>
+      </c>
+      <c r="EE2" s="43" t="s">
+        <v>528</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added sheets in demo testData.xslx and modified url of automation for FileUpload in testData.xslx
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation/TestData/TestData.xlsx
+++ b/src/main/resources/config/automation/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15672" windowHeight="8976" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="8970" firstSheet="11" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="S181372" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2226" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2226" uniqueCount="566">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1724,6 +1724,9 @@
   </si>
   <si>
     <t>ALLWOAGCO</t>
+  </si>
+  <si>
+    <t>http://ech-10-168-128-251.mastercard.int:25003/integratedIssuing-customerPortal/mpts/app/Login</t>
   </si>
 </sst>
 </file>
@@ -2303,20 +2306,20 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.5546875" customWidth="1"/>
+    <col min="1" max="1" width="44.5703125" customWidth="1"/>
     <col min="2" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" customWidth="1"/>
-    <col min="9" max="9" width="11.21875" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1"/>
-    <col min="11" max="11" width="25.33203125" customWidth="1"/>
-    <col min="12" max="13" width="15.5546875" customWidth="1"/>
-    <col min="15" max="15" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" customWidth="1"/>
+    <col min="12" max="13" width="15.5703125" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:63" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2507,7 +2510,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:63" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2694,7 +2697,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:63" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -2883,12 +2886,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -2942,7 +2945,7 @@
       </c>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>301</v>
       </c>
@@ -2995,7 +2998,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>302</v>
       </c>
@@ -3048,7 +3051,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>303</v>
       </c>
@@ -3101,7 +3104,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>304</v>
       </c>
@@ -3154,7 +3157,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>305</v>
       </c>
@@ -3220,18 +3223,18 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.77734375" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.77734375" style="33" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="33" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" style="33" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="31"/>
+    <col min="1" max="1" width="61.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="33" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="33" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="33" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3251,7 +3254,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>382</v>
       </c>
@@ -3271,7 +3274,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>383</v>
       </c>
@@ -3291,7 +3294,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>390</v>
       </c>
@@ -3311,7 +3314,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>384</v>
       </c>
@@ -3331,7 +3334,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>385</v>
       </c>
@@ -3351,7 +3354,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>386</v>
       </c>
@@ -3371,7 +3374,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>387</v>
       </c>
@@ -3404,26 +3407,27 @@
       <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" style="24" customWidth="1"/>
-    <col min="2" max="2" width="22.77734375" style="24" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" style="24" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" style="24" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="24" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="24" customWidth="1"/>
     <col min="5" max="5" width="15" style="24" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="24" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" style="24" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="24"/>
-    <col min="10" max="10" width="9.6640625" style="24" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" style="24" customWidth="1"/>
-    <col min="12" max="12" width="20.21875" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="24" customWidth="1"/>
-    <col min="14" max="14" width="20.21875" style="24" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="24"/>
+    <col min="6" max="6" width="14.7109375" style="24" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="24" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="24"/>
+    <col min="10" max="10" width="9.7109375" style="24" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="24" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" style="24" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="9.140625" customWidth="1"/>
+    <col min="18" max="16384" width="8.85546875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -3470,7 +3474,7 @@
       <c r="P1" s="24"/>
       <c r="Q1" s="24"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>317</v>
       </c>
@@ -3513,17 +3517,17 @@
       <c r="P2" s="24"/>
       <c r="Q2" s="24"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O3" s="24"/>
       <c r="P3" s="24"/>
       <c r="Q3" s="24"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O4" s="24"/>
       <c r="P4" s="24"/>
       <c r="Q4" s="24"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O13" s="24"/>
       <c r="P13" s="24"/>
       <c r="Q13" s="24"/>
@@ -3541,24 +3545,24 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.109375" style="24" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="24" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" style="24" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="24" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="24" customWidth="1"/>
     <col min="4" max="5" width="15" style="24" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="24" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="24" customWidth="1"/>
     <col min="7" max="7" width="15" style="24" customWidth="1"/>
-    <col min="8" max="8" width="19.21875" style="24" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" style="24" customWidth="1"/>
     <col min="9" max="9" width="15" style="24" customWidth="1"/>
-    <col min="10" max="12" width="9.21875" style="24" customWidth="1"/>
-    <col min="13" max="13" width="28.77734375" style="24" customWidth="1"/>
-    <col min="14" max="14" width="11.77734375" style="24" customWidth="1"/>
-    <col min="15" max="15" width="18.77734375" style="24" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="24"/>
+    <col min="10" max="12" width="9.28515625" style="24" customWidth="1"/>
+    <col min="13" max="13" width="28.7109375" style="24" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" style="24" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" style="24" customWidth="1"/>
+    <col min="16" max="16384" width="8.85546875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -3605,7 +3609,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>334</v>
       </c>
@@ -3646,7 +3650,7 @@
       <c r="N2" s="25"/>
       <c r="O2" s="25"/>
     </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>340</v>
       </c>
@@ -3700,20 +3704,20 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="16.21875" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -3748,7 +3752,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>345</v>
       </c>
@@ -3804,14 +3808,14 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="75" max="75" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="75" max="75" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:135" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:135" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -4218,7 +4222,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:135" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:135" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>483</v>
       </c>
@@ -4605,19 +4609,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EE2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:135" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:135" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -5024,12 +5028,12 @@
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:135" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:135" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>530</v>
       </c>
       <c r="B2" t="s">
-        <v>523</v>
+        <v>565</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>524</v>
@@ -5414,22 +5418,22 @@
       <selection activeCell="BR2" sqref="BR2:BR8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.109375" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="19" max="19" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="7.44140625" customWidth="1"/>
-    <col min="66" max="66" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="17.5546875" customWidth="1"/>
-    <col min="97" max="97" width="10.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="7.42578125" customWidth="1"/>
+    <col min="66" max="66" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="17.5703125" customWidth="1"/>
+    <col min="97" max="97" width="10.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:118" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:118" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -5783,7 +5787,7 @@
       </c>
       <c r="DN1" s="4"/>
     </row>
-    <row r="2" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:118" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>132</v>
       </c>
@@ -6110,7 +6114,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="3" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:118" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>140</v>
       </c>
@@ -6389,7 +6393,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:118" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:118" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>150</v>
       </c>
@@ -6668,7 +6672,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:118" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>156</v>
       </c>
@@ -6947,7 +6951,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:118" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>163</v>
       </c>
@@ -7226,7 +7230,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:118" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>169</v>
       </c>
@@ -7507,7 +7511,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:118" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>175</v>
       </c>
@@ -7788,7 +7792,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:118" x14ac:dyDescent="0.25">
       <c r="CS9"/>
       <c r="CT9" t="s">
         <v>162</v>
@@ -7797,7 +7801,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:118" x14ac:dyDescent="0.25">
       <c r="CS10"/>
       <c r="CT10" t="s">
         <v>162</v>
@@ -7806,7 +7810,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:118" x14ac:dyDescent="0.25">
       <c r="CS11"/>
       <c r="CT11" t="s">
         <v>162</v>
@@ -7815,502 +7819,502 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:118" x14ac:dyDescent="0.25">
       <c r="CS12"/>
     </row>
-    <row r="13" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:118" x14ac:dyDescent="0.25">
       <c r="CS13"/>
     </row>
-    <row r="14" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:118" x14ac:dyDescent="0.25">
       <c r="CS14"/>
     </row>
-    <row r="15" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:118" x14ac:dyDescent="0.25">
       <c r="CS15"/>
     </row>
-    <row r="16" spans="1:118" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:118" x14ac:dyDescent="0.25">
       <c r="CS16"/>
     </row>
-    <row r="17" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="17" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS17"/>
     </row>
-    <row r="18" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="18" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS18"/>
     </row>
-    <row r="19" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="19" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS19"/>
     </row>
-    <row r="20" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="20" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS20"/>
     </row>
-    <row r="21" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="21" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS21"/>
     </row>
-    <row r="22" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="22" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS22"/>
     </row>
-    <row r="23" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="23" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS23"/>
     </row>
-    <row r="24" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="24" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS24"/>
     </row>
-    <row r="25" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="25" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS25"/>
     </row>
-    <row r="26" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="26" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS26"/>
     </row>
-    <row r="27" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="27" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS27"/>
     </row>
-    <row r="28" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="28" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS28"/>
     </row>
-    <row r="29" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="29" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS29"/>
     </row>
-    <row r="30" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="30" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS30"/>
     </row>
-    <row r="31" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="31" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS31"/>
     </row>
-    <row r="32" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="32" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS32"/>
     </row>
-    <row r="33" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="33" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS33"/>
     </row>
-    <row r="34" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="34" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS34"/>
     </row>
-    <row r="35" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="35" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS35"/>
     </row>
-    <row r="36" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="36" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS36"/>
     </row>
-    <row r="37" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="37" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS37"/>
     </row>
-    <row r="38" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="38" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS38"/>
     </row>
-    <row r="39" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="39" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS39"/>
     </row>
-    <row r="40" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="40" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS40"/>
     </row>
-    <row r="41" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="41" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS41"/>
     </row>
-    <row r="42" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="42" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS42"/>
     </row>
-    <row r="43" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="43" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS43"/>
     </row>
-    <row r="44" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="44" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS44"/>
     </row>
-    <row r="45" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="45" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS45"/>
     </row>
-    <row r="46" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="46" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS46"/>
     </row>
-    <row r="47" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="47" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS47"/>
     </row>
-    <row r="48" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="48" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS48"/>
     </row>
-    <row r="49" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="49" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS49"/>
     </row>
-    <row r="50" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="50" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS50"/>
     </row>
-    <row r="51" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="51" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS51"/>
     </row>
-    <row r="52" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="52" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS52"/>
     </row>
-    <row r="53" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="53" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS53"/>
     </row>
-    <row r="54" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="54" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS54"/>
     </row>
-    <row r="55" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="55" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS55"/>
     </row>
-    <row r="56" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="56" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS56"/>
     </row>
-    <row r="57" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="57" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS57"/>
     </row>
-    <row r="58" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="58" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS58"/>
     </row>
-    <row r="59" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="59" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS59"/>
     </row>
-    <row r="60" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="60" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS60"/>
     </row>
-    <row r="61" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="61" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS61"/>
     </row>
-    <row r="62" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="62" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS62"/>
     </row>
-    <row r="63" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="63" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS63"/>
     </row>
-    <row r="64" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="64" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS64"/>
     </row>
-    <row r="65" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="65" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS65"/>
     </row>
-    <row r="66" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="66" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS66"/>
     </row>
-    <row r="67" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="67" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS67"/>
     </row>
-    <row r="68" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="68" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS68"/>
     </row>
-    <row r="69" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="69" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS69"/>
     </row>
-    <row r="70" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="70" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS70"/>
     </row>
-    <row r="71" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="71" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS71"/>
     </row>
-    <row r="72" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="72" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS72"/>
     </row>
-    <row r="73" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="73" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS73"/>
     </row>
-    <row r="74" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="74" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS74"/>
     </row>
-    <row r="75" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="75" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS75"/>
     </row>
-    <row r="76" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="76" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS76"/>
     </row>
-    <row r="77" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="77" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS77"/>
     </row>
-    <row r="78" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="78" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS78"/>
     </row>
-    <row r="79" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="79" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS79"/>
     </row>
-    <row r="80" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="80" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS80"/>
     </row>
-    <row r="81" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="81" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS81"/>
     </row>
-    <row r="82" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="82" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS82"/>
     </row>
-    <row r="83" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="83" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS83"/>
     </row>
-    <row r="84" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="84" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS84"/>
     </row>
-    <row r="85" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="85" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS85"/>
     </row>
-    <row r="86" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="86" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS86"/>
     </row>
-    <row r="87" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="87" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS87"/>
     </row>
-    <row r="88" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="88" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS88"/>
     </row>
-    <row r="89" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="89" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS89"/>
     </row>
-    <row r="90" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="90" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS90"/>
     </row>
-    <row r="91" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="91" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS91"/>
     </row>
-    <row r="92" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="92" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS92"/>
     </row>
-    <row r="93" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="93" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS93"/>
     </row>
-    <row r="94" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="94" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS94"/>
     </row>
-    <row r="95" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="95" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS95"/>
     </row>
-    <row r="96" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="96" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS96"/>
     </row>
-    <row r="97" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="97" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS97"/>
     </row>
-    <row r="98" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="98" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS98"/>
     </row>
-    <row r="99" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="99" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS99"/>
     </row>
-    <row r="100" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="100" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS100"/>
     </row>
-    <row r="101" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="101" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS101"/>
     </row>
-    <row r="102" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="102" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS102"/>
     </row>
-    <row r="103" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="103" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS103"/>
     </row>
-    <row r="104" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="104" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS104"/>
     </row>
-    <row r="105" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="105" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS105"/>
     </row>
-    <row r="106" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="106" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS106"/>
     </row>
-    <row r="107" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="107" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS107"/>
     </row>
-    <row r="108" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="108" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS108"/>
     </row>
-    <row r="109" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="109" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS109"/>
     </row>
-    <row r="110" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="110" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS110"/>
     </row>
-    <row r="111" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="111" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS111"/>
     </row>
-    <row r="112" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="112" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS112"/>
     </row>
-    <row r="113" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="113" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS113"/>
     </row>
-    <row r="114" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="114" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS114"/>
     </row>
-    <row r="115" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="115" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS115"/>
     </row>
-    <row r="116" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="116" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS116"/>
     </row>
-    <row r="117" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="117" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS117"/>
     </row>
-    <row r="118" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="118" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS118"/>
     </row>
-    <row r="119" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="119" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS119"/>
     </row>
-    <row r="120" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="120" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS120"/>
     </row>
-    <row r="121" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="121" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS121"/>
     </row>
-    <row r="122" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="122" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS122"/>
     </row>
-    <row r="123" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="123" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS123"/>
     </row>
-    <row r="124" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="124" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS124"/>
     </row>
-    <row r="125" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="125" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS125"/>
     </row>
-    <row r="126" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="126" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS126"/>
     </row>
-    <row r="127" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="127" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS127"/>
     </row>
-    <row r="128" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="128" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS128"/>
     </row>
-    <row r="129" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="129" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS129"/>
     </row>
-    <row r="130" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="130" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS130"/>
     </row>
-    <row r="131" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="131" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS131"/>
     </row>
-    <row r="132" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="132" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS132"/>
     </row>
-    <row r="133" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="133" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS133"/>
     </row>
-    <row r="134" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="134" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS134"/>
     </row>
-    <row r="135" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="135" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS135"/>
     </row>
-    <row r="136" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="136" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS136"/>
     </row>
-    <row r="137" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="137" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS137"/>
     </row>
-    <row r="138" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="138" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS138"/>
     </row>
-    <row r="139" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="139" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS139"/>
     </row>
-    <row r="140" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="140" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS140"/>
     </row>
-    <row r="141" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="141" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS141"/>
     </row>
-    <row r="142" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="142" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS142"/>
     </row>
-    <row r="143" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="143" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS143"/>
     </row>
-    <row r="144" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="144" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS144"/>
     </row>
-    <row r="145" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="145" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS145"/>
     </row>
-    <row r="146" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="146" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS146"/>
     </row>
-    <row r="147" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="147" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS147"/>
     </row>
-    <row r="148" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="148" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS148"/>
     </row>
-    <row r="149" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="149" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS149"/>
     </row>
-    <row r="150" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="150" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS150"/>
     </row>
-    <row r="151" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="151" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS151"/>
     </row>
-    <row r="152" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="152" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS152"/>
     </row>
-    <row r="153" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="153" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS153"/>
     </row>
-    <row r="154" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="154" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS154"/>
     </row>
-    <row r="155" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="155" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS155"/>
     </row>
-    <row r="156" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="156" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS156"/>
     </row>
-    <row r="157" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="157" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS157"/>
     </row>
-    <row r="158" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="158" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS158"/>
     </row>
-    <row r="159" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="159" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS159"/>
     </row>
-    <row r="160" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="160" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS160"/>
     </row>
-    <row r="161" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="161" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS161"/>
     </row>
-    <row r="162" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="162" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS162"/>
     </row>
-    <row r="163" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="163" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS163"/>
     </row>
-    <row r="164" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="164" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS164"/>
     </row>
-    <row r="165" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="165" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS165"/>
     </row>
-    <row r="166" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="166" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS166"/>
     </row>
-    <row r="167" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="167" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS167"/>
     </row>
-    <row r="168" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="168" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS168"/>
     </row>
-    <row r="169" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="169" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS169"/>
     </row>
-    <row r="170" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="170" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS170"/>
     </row>
-    <row r="171" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="171" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS171"/>
     </row>
-    <row r="172" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="172" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS172"/>
     </row>
-    <row r="173" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="173" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS173"/>
     </row>
-    <row r="174" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="174" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS174"/>
     </row>
-    <row r="175" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="175" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS175"/>
     </row>
-    <row r="176" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="176" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS176"/>
     </row>
-    <row r="177" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="177" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS177"/>
     </row>
   </sheetData>
@@ -8327,17 +8331,17 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.21875" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="43.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -8372,7 +8376,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>186</v>
       </c>
@@ -8399,7 +8403,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>190</v>
       </c>
@@ -8430,7 +8434,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>191</v>
       </c>
@@ -8451,7 +8455,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>192</v>
       </c>
@@ -8487,19 +8491,19 @@
       <selection sqref="A1:Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="52" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="9" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.6640625" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" customWidth="1"/>
     <col min="17" max="17" width="47" customWidth="1"/>
-    <col min="18" max="18" width="37.6640625" customWidth="1"/>
+    <col min="18" max="18" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8550,7 +8554,7 @@
       </c>
       <c r="R1" s="20"/>
     </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>201</v>
       </c>
@@ -8601,7 +8605,7 @@
       </c>
       <c r="R2" s="18"/>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>201</v>
       </c>
@@ -8652,7 +8656,7 @@
       </c>
       <c r="R3" s="16"/>
     </row>
-    <row r="4" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>201</v>
       </c>
@@ -8703,7 +8707,7 @@
       </c>
       <c r="R4" s="17"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>201</v>
       </c>
@@ -8754,7 +8758,7 @@
       </c>
       <c r="R5" s="16"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>201</v>
       </c>
@@ -8818,13 +8822,13 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.88671875" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -8844,7 +8848,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>258</v>
       </c>
@@ -8864,7 +8868,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>262</v>
       </c>
@@ -8895,12 +8899,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -8929,7 +8933,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>264</v>
       </c>
@@ -8969,12 +8973,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="34.6640625" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -8997,7 +9001,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>268</v>
       </c>
@@ -9020,7 +9024,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>272</v>
       </c>
@@ -9041,7 +9045,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>274</v>
       </c>
@@ -9073,14 +9077,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -9100,7 +9104,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>258</v>
       </c>
@@ -9120,7 +9124,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>262</v>
       </c>
@@ -9149,39 +9153,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="BD1" sqref="BD1:DS1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5546875" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="28.5546875" customWidth="1"/>
-    <col min="23" max="23" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="28.5703125" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
@@ -9348,7 +9352,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="2" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>538</v>
       </c>
@@ -9509,7 +9513,7 @@
       </c>
       <c r="BC2" s="47"/>
     </row>
-    <row r="3" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>546</v>
       </c>
@@ -9668,7 +9672,7 @@
       <c r="BB3" s="47"/>
       <c r="BC3" s="47"/>
     </row>
-    <row r="4" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>548</v>
       </c>
@@ -9827,7 +9831,7 @@
       <c r="BB4" s="47"/>
       <c r="BC4" s="47"/>
     </row>
-    <row r="5" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
         <v>550</v>
       </c>
@@ -9988,7 +9992,7 @@
       </c>
       <c r="BC5" s="47"/>
     </row>
-    <row r="6" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
         <v>553</v>
       </c>
@@ -10149,7 +10153,7 @@
       </c>
       <c r="BC6" s="47"/>
     </row>
-    <row r="7" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
         <v>555</v>
       </c>
@@ -10310,7 +10314,7 @@
       </c>
       <c r="BC7" s="47"/>
     </row>
-    <row r="8" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
         <v>557</v>
       </c>
@@ -10471,7 +10475,7 @@
       </c>
       <c r="BC8" s="47"/>
     </row>
-    <row r="9" spans="1:55" s="50" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:55" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
         <v>559</v>
       </c>
@@ -10630,7 +10634,7 @@
       <c r="BB9" s="47"/>
       <c r="BC9" s="47"/>
     </row>
-    <row r="10" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>561</v>
       </c>
@@ -10789,7 +10793,7 @@
       <c r="BB10" s="47"/>
       <c r="BC10" s="47"/>
     </row>
-    <row r="11" spans="1:55" s="50" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:55" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
         <v>563</v>
       </c>

</xml_diff>

<commit_message>
Committing Changes of File upload of device type Static Virtual Card.
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation/TestData/TestData.xlsx
+++ b/src/main/resources/config/automation/TestData/TestData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2226" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2228" uniqueCount="568">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1727,6 +1727,12 @@
   </si>
   <si>
     <t>http://ech-10-168-128-251.mastercard.int:25003/integratedIssuing-customerPortal/mpts/app/Login</t>
+  </si>
+  <si>
+    <t>WalletPlancode</t>
+  </si>
+  <si>
+    <t>WalletPlanDescription</t>
   </si>
 </sst>
 </file>
@@ -4607,10 +4613,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EE2"/>
+  <dimension ref="A1:EG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="DP1" workbookViewId="0">
+      <selection activeCell="ED1" sqref="ED1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4621,7 +4627,7 @@
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:135" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:137" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -5022,13 +5028,19 @@
         <v>480</v>
       </c>
       <c r="ED1" s="36" t="s">
+        <v>567</v>
+      </c>
+      <c r="EE1" s="36" t="s">
+        <v>566</v>
+      </c>
+      <c r="EF1" s="36" t="s">
         <v>481</v>
       </c>
-      <c r="EE1" s="36" t="s">
+      <c r="EG1" s="36" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:135" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:137" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>530</v>
       </c>
@@ -5398,10 +5410,12 @@
       <c r="EC2" s="42" t="s">
         <v>518</v>
       </c>
-      <c r="ED2" s="42" t="s">
+      <c r="ED2" s="42"/>
+      <c r="EE2" s="42"/>
+      <c r="EF2" s="42" t="s">
         <v>519</v>
       </c>
-      <c r="EE2" s="41" t="s">
+      <c r="EG2" s="41" t="s">
         <v>520</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revamping Files for File upload scenarios
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation/TestData/TestData.xlsx
+++ b/src/main/resources/config/automation/TestData/TestData.xlsx
@@ -4652,8 +4652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EM3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="CB1" workbookViewId="0">
+      <selection activeCell="CP3" sqref="CP3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5359,7 +5359,7 @@
         <v>502</v>
       </c>
       <c r="CP2" s="40" t="s">
-        <v>355</v>
+        <v>492</v>
       </c>
       <c r="CQ2" s="11" t="s">
         <v>48</v>
@@ -5744,7 +5744,7 @@
         <v>502</v>
       </c>
       <c r="CP3" s="40" t="s">
-        <v>355</v>
+        <v>492</v>
       </c>
       <c r="CQ3" s="11" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Changes made for File upload scenarios, and adding additional fields required for Automation and Automation2.
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation/TestData/TestData.xlsx
+++ b/src/main/resources/config/automation/TestData/TestData.xlsx
@@ -4652,8 +4652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EM3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CB1" workbookViewId="0">
-      <selection activeCell="CP3" sqref="CP3"/>
+    <sheetView tabSelected="1" topLeftCell="DL1" workbookViewId="0">
+      <selection activeCell="EB13" sqref="EB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added script for adding high risk country
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation/TestData/TestData.xlsx
+++ b/src/main/resources/config/automation/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="8970" firstSheet="11" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15672" windowHeight="8976" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="S181372" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2351" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2395" uniqueCount="587">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1769,6 +1769,27 @@
   </si>
   <si>
     <t>http://ech-10-168-128-251.mastercard.int:25003/integratedIssuing-customerPortal/mtps/app/Login</t>
+  </si>
+  <si>
+    <t>HighRiskCountry</t>
+  </si>
+  <si>
+    <t>TaxOnIncomeFeeType</t>
+  </si>
+  <si>
+    <t>TaxOnIncomeStatus</t>
+  </si>
+  <si>
+    <t>MccCode</t>
+  </si>
+  <si>
+    <t>CANADA [124]</t>
+  </si>
+  <si>
+    <t>Loan Processing Fee [44]</t>
+  </si>
+  <si>
+    <t>Accounting, Auditing, and Bookkeeping Services [8931]</t>
   </si>
 </sst>
 </file>
@@ -2349,20 +2370,20 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.5703125" customWidth="1"/>
+    <col min="1" max="1" width="44.5546875" customWidth="1"/>
     <col min="2" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="25.28515625" customWidth="1"/>
-    <col min="12" max="13" width="15.5703125" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="11" max="11" width="25.33203125" customWidth="1"/>
+    <col min="12" max="13" width="15.5546875" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2553,7 +2574,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2740,7 +2761,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:63" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -2929,12 +2950,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -2988,7 +3009,7 @@
       </c>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>301</v>
       </c>
@@ -3041,7 +3062,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>302</v>
       </c>
@@ -3094,7 +3115,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>303</v>
       </c>
@@ -3147,7 +3168,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>304</v>
       </c>
@@ -3200,7 +3221,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>305</v>
       </c>
@@ -3266,18 +3287,18 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" style="33" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="33" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="33" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="31"/>
+    <col min="1" max="1" width="61.6640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="33" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="33" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3297,7 +3318,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>382</v>
       </c>
@@ -3317,7 +3338,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>383</v>
       </c>
@@ -3337,7 +3358,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
         <v>390</v>
       </c>
@@ -3357,7 +3378,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
         <v>384</v>
       </c>
@@ -3377,7 +3398,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
         <v>385</v>
       </c>
@@ -3397,7 +3418,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>386</v>
       </c>
@@ -3417,7 +3438,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
         <v>387</v>
       </c>
@@ -3450,27 +3471,27 @@
       <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" style="24" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" style="24" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="24" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="24" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="24" customWidth="1"/>
     <col min="5" max="5" width="15" style="24" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="24" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="24" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="24"/>
-    <col min="10" max="10" width="9.7109375" style="24" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" style="24" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" style="24" customWidth="1"/>
-    <col min="14" max="14" width="20.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="9.140625" customWidth="1"/>
-    <col min="18" max="16384" width="8.85546875" style="24"/>
+    <col min="6" max="6" width="14.6640625" style="24" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" style="24" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="24"/>
+    <col min="10" max="10" width="9.6640625" style="24" customWidth="1"/>
+    <col min="11" max="11" width="8.5546875" style="24" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="24" customWidth="1"/>
+    <col min="14" max="14" width="20.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="9.109375" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -3517,7 +3538,7 @@
       <c r="P1" s="24"/>
       <c r="Q1" s="24"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>317</v>
       </c>
@@ -3560,17 +3581,17 @@
       <c r="P2" s="24"/>
       <c r="Q2" s="24"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="O3" s="24"/>
       <c r="P3" s="24"/>
       <c r="Q3" s="24"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="O4" s="24"/>
       <c r="P4" s="24"/>
       <c r="Q4" s="24"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="O13" s="24"/>
       <c r="P13" s="24"/>
       <c r="Q13" s="24"/>
@@ -3588,24 +3609,24 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.140625" style="24" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="24" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="24" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" style="24" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="24" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="24" customWidth="1"/>
     <col min="4" max="5" width="15" style="24" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="24" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="24" customWidth="1"/>
     <col min="7" max="7" width="15" style="24" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" style="24" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" style="24" customWidth="1"/>
     <col min="9" max="9" width="15" style="24" customWidth="1"/>
-    <col min="10" max="12" width="9.28515625" style="24" customWidth="1"/>
-    <col min="13" max="13" width="28.7109375" style="24" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" style="24" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" style="24" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="24"/>
+    <col min="10" max="12" width="9.33203125" style="24" customWidth="1"/>
+    <col min="13" max="13" width="28.6640625" style="24" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" style="24" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" style="24" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -3652,7 +3673,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>334</v>
       </c>
@@ -3693,7 +3714,7 @@
       <c r="N2" s="25"/>
       <c r="O2" s="25"/>
     </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>340</v>
       </c>
@@ -3747,20 +3768,20 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -3795,7 +3816,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>345</v>
       </c>
@@ -3851,14 +3872,14 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="75" max="75" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="75" max="75" width="28.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:135" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:135" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -4265,7 +4286,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:135" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:135" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>483</v>
       </c>
@@ -4652,20 +4673,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EM3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DL1" workbookViewId="0">
+    <sheetView topLeftCell="DL1" workbookViewId="0">
       <selection activeCell="EB13" sqref="EB13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:143" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:143" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -5096,7 +5117,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:143" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:143" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>530</v>
       </c>
@@ -5481,7 +5502,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="3" spans="1:143" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:143" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>568</v>
       </c>
@@ -5891,22 +5912,22 @@
       <selection activeCell="BR2" sqref="BR2:BR8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="7.42578125" customWidth="1"/>
-    <col min="66" max="66" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="17.5703125" customWidth="1"/>
-    <col min="97" max="97" width="10.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="37.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="7.44140625" customWidth="1"/>
+    <col min="66" max="66" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="17.5546875" customWidth="1"/>
+    <col min="97" max="97" width="10.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:118" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:118" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -6260,7 +6281,7 @@
       </c>
       <c r="DN1" s="4"/>
     </row>
-    <row r="2" spans="1:118" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>132</v>
       </c>
@@ -6587,7 +6608,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="3" spans="1:118" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>140</v>
       </c>
@@ -6866,7 +6887,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:118" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:118" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>150</v>
       </c>
@@ -7145,7 +7166,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:118" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>156</v>
       </c>
@@ -7424,7 +7445,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:118" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>163</v>
       </c>
@@ -7703,7 +7724,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:118" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>169</v>
       </c>
@@ -7984,7 +8005,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:118" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>175</v>
       </c>
@@ -8265,7 +8286,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:118" x14ac:dyDescent="0.3">
       <c r="CS9"/>
       <c r="CT9" t="s">
         <v>162</v>
@@ -8274,7 +8295,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:118" x14ac:dyDescent="0.3">
       <c r="CS10"/>
       <c r="CT10" t="s">
         <v>162</v>
@@ -8283,7 +8304,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:118" x14ac:dyDescent="0.3">
       <c r="CS11"/>
       <c r="CT11" t="s">
         <v>162</v>
@@ -8292,502 +8313,502 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:118" x14ac:dyDescent="0.3">
       <c r="CS12"/>
     </row>
-    <row r="13" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:118" x14ac:dyDescent="0.3">
       <c r="CS13"/>
     </row>
-    <row r="14" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:118" x14ac:dyDescent="0.3">
       <c r="CS14"/>
     </row>
-    <row r="15" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:118" x14ac:dyDescent="0.3">
       <c r="CS15"/>
     </row>
-    <row r="16" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:118" x14ac:dyDescent="0.3">
       <c r="CS16"/>
     </row>
-    <row r="17" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="17" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS17"/>
     </row>
-    <row r="18" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="18" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS18"/>
     </row>
-    <row r="19" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="19" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS19"/>
     </row>
-    <row r="20" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="20" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS20"/>
     </row>
-    <row r="21" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="21" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS21"/>
     </row>
-    <row r="22" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="22" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS22"/>
     </row>
-    <row r="23" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="23" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS23"/>
     </row>
-    <row r="24" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="24" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS24"/>
     </row>
-    <row r="25" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="25" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS25"/>
     </row>
-    <row r="26" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="26" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS26"/>
     </row>
-    <row r="27" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="27" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS27"/>
     </row>
-    <row r="28" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="28" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS28"/>
     </row>
-    <row r="29" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="29" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS29"/>
     </row>
-    <row r="30" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="30" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS30"/>
     </row>
-    <row r="31" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="31" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS31"/>
     </row>
-    <row r="32" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="32" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS32"/>
     </row>
-    <row r="33" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="33" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS33"/>
     </row>
-    <row r="34" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="34" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS34"/>
     </row>
-    <row r="35" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="35" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS35"/>
     </row>
-    <row r="36" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="36" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS36"/>
     </row>
-    <row r="37" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="37" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS37"/>
     </row>
-    <row r="38" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="38" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS38"/>
     </row>
-    <row r="39" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="39" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS39"/>
     </row>
-    <row r="40" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="40" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS40"/>
     </row>
-    <row r="41" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="41" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS41"/>
     </row>
-    <row r="42" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="42" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS42"/>
     </row>
-    <row r="43" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="43" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS43"/>
     </row>
-    <row r="44" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="44" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS44"/>
     </row>
-    <row r="45" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="45" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS45"/>
     </row>
-    <row r="46" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="46" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS46"/>
     </row>
-    <row r="47" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="47" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS47"/>
     </row>
-    <row r="48" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="48" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS48"/>
     </row>
-    <row r="49" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="49" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS49"/>
     </row>
-    <row r="50" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="50" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS50"/>
     </row>
-    <row r="51" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="51" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS51"/>
     </row>
-    <row r="52" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="52" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS52"/>
     </row>
-    <row r="53" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="53" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS53"/>
     </row>
-    <row r="54" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="54" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS54"/>
     </row>
-    <row r="55" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="55" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS55"/>
     </row>
-    <row r="56" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="56" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS56"/>
     </row>
-    <row r="57" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="57" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS57"/>
     </row>
-    <row r="58" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="58" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS58"/>
     </row>
-    <row r="59" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="59" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS59"/>
     </row>
-    <row r="60" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="60" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS60"/>
     </row>
-    <row r="61" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="61" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS61"/>
     </row>
-    <row r="62" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="62" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS62"/>
     </row>
-    <row r="63" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="63" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS63"/>
     </row>
-    <row r="64" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="64" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS64"/>
     </row>
-    <row r="65" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="65" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS65"/>
     </row>
-    <row r="66" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="66" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS66"/>
     </row>
-    <row r="67" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="67" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS67"/>
     </row>
-    <row r="68" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="68" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS68"/>
     </row>
-    <row r="69" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="69" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS69"/>
     </row>
-    <row r="70" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="70" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS70"/>
     </row>
-    <row r="71" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="71" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS71"/>
     </row>
-    <row r="72" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="72" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS72"/>
     </row>
-    <row r="73" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="73" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS73"/>
     </row>
-    <row r="74" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="74" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS74"/>
     </row>
-    <row r="75" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="75" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS75"/>
     </row>
-    <row r="76" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="76" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS76"/>
     </row>
-    <row r="77" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="77" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS77"/>
     </row>
-    <row r="78" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="78" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS78"/>
     </row>
-    <row r="79" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="79" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS79"/>
     </row>
-    <row r="80" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="80" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS80"/>
     </row>
-    <row r="81" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="81" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS81"/>
     </row>
-    <row r="82" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="82" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS82"/>
     </row>
-    <row r="83" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="83" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS83"/>
     </row>
-    <row r="84" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="84" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS84"/>
     </row>
-    <row r="85" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="85" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS85"/>
     </row>
-    <row r="86" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="86" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS86"/>
     </row>
-    <row r="87" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="87" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS87"/>
     </row>
-    <row r="88" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="88" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS88"/>
     </row>
-    <row r="89" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="89" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS89"/>
     </row>
-    <row r="90" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="90" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS90"/>
     </row>
-    <row r="91" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="91" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS91"/>
     </row>
-    <row r="92" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="92" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS92"/>
     </row>
-    <row r="93" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="93" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS93"/>
     </row>
-    <row r="94" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="94" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS94"/>
     </row>
-    <row r="95" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="95" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS95"/>
     </row>
-    <row r="96" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="96" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS96"/>
     </row>
-    <row r="97" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="97" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS97"/>
     </row>
-    <row r="98" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="98" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS98"/>
     </row>
-    <row r="99" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="99" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS99"/>
     </row>
-    <row r="100" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="100" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS100"/>
     </row>
-    <row r="101" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="101" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS101"/>
     </row>
-    <row r="102" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="102" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS102"/>
     </row>
-    <row r="103" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="103" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS103"/>
     </row>
-    <row r="104" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="104" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS104"/>
     </row>
-    <row r="105" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="105" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS105"/>
     </row>
-    <row r="106" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="106" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS106"/>
     </row>
-    <row r="107" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="107" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS107"/>
     </row>
-    <row r="108" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="108" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS108"/>
     </row>
-    <row r="109" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="109" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS109"/>
     </row>
-    <row r="110" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="110" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS110"/>
     </row>
-    <row r="111" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="111" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS111"/>
     </row>
-    <row r="112" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="112" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS112"/>
     </row>
-    <row r="113" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="113" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS113"/>
     </row>
-    <row r="114" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="114" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS114"/>
     </row>
-    <row r="115" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="115" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS115"/>
     </row>
-    <row r="116" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="116" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS116"/>
     </row>
-    <row r="117" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="117" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS117"/>
     </row>
-    <row r="118" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="118" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS118"/>
     </row>
-    <row r="119" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="119" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS119"/>
     </row>
-    <row r="120" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="120" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS120"/>
     </row>
-    <row r="121" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="121" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS121"/>
     </row>
-    <row r="122" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="122" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS122"/>
     </row>
-    <row r="123" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="123" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS123"/>
     </row>
-    <row r="124" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="124" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS124"/>
     </row>
-    <row r="125" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="125" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS125"/>
     </row>
-    <row r="126" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="126" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS126"/>
     </row>
-    <row r="127" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="127" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS127"/>
     </row>
-    <row r="128" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="128" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS128"/>
     </row>
-    <row r="129" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="129" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS129"/>
     </row>
-    <row r="130" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="130" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS130"/>
     </row>
-    <row r="131" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="131" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS131"/>
     </row>
-    <row r="132" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="132" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS132"/>
     </row>
-    <row r="133" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="133" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS133"/>
     </row>
-    <row r="134" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="134" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS134"/>
     </row>
-    <row r="135" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="135" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS135"/>
     </row>
-    <row r="136" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="136" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS136"/>
     </row>
-    <row r="137" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="137" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS137"/>
     </row>
-    <row r="138" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="138" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS138"/>
     </row>
-    <row r="139" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="139" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS139"/>
     </row>
-    <row r="140" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="140" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS140"/>
     </row>
-    <row r="141" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="141" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS141"/>
     </row>
-    <row r="142" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="142" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS142"/>
     </row>
-    <row r="143" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="143" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS143"/>
     </row>
-    <row r="144" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="144" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS144"/>
     </row>
-    <row r="145" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="145" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS145"/>
     </row>
-    <row r="146" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="146" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS146"/>
     </row>
-    <row r="147" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="147" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS147"/>
     </row>
-    <row r="148" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="148" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS148"/>
     </row>
-    <row r="149" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="149" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS149"/>
     </row>
-    <row r="150" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="150" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS150"/>
     </row>
-    <row r="151" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="151" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS151"/>
     </row>
-    <row r="152" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="152" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS152"/>
     </row>
-    <row r="153" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="153" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS153"/>
     </row>
-    <row r="154" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="154" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS154"/>
     </row>
-    <row r="155" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="155" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS155"/>
     </row>
-    <row r="156" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="156" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS156"/>
     </row>
-    <row r="157" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="157" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS157"/>
     </row>
-    <row r="158" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="158" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS158"/>
     </row>
-    <row r="159" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="159" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS159"/>
     </row>
-    <row r="160" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="160" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS160"/>
     </row>
-    <row r="161" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="161" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS161"/>
     </row>
-    <row r="162" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="162" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS162"/>
     </row>
-    <row r="163" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="163" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS163"/>
     </row>
-    <row r="164" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="164" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS164"/>
     </row>
-    <row r="165" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="165" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS165"/>
     </row>
-    <row r="166" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="166" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS166"/>
     </row>
-    <row r="167" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="167" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS167"/>
     </row>
-    <row r="168" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="168" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS168"/>
     </row>
-    <row r="169" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="169" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS169"/>
     </row>
-    <row r="170" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="170" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS170"/>
     </row>
-    <row r="171" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="171" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS171"/>
     </row>
-    <row r="172" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="172" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS172"/>
     </row>
-    <row r="173" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="173" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS173"/>
     </row>
-    <row r="174" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="174" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS174"/>
     </row>
-    <row r="175" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="175" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS175"/>
     </row>
-    <row r="176" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="176" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS176"/>
     </row>
-    <row r="177" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="177" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS177"/>
     </row>
   </sheetData>
@@ -8804,17 +8825,17 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -8849,7 +8870,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>186</v>
       </c>
@@ -8876,7 +8897,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>190</v>
       </c>
@@ -8907,7 +8928,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>191</v>
       </c>
@@ -8928,7 +8949,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>192</v>
       </c>
@@ -8964,19 +8985,19 @@
       <selection sqref="A1:Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="7" max="7" width="52" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="9" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.7109375" customWidth="1"/>
+    <col min="16" max="16" width="20.6640625" customWidth="1"/>
     <col min="17" max="17" width="47" customWidth="1"/>
-    <col min="18" max="18" width="37.7109375" customWidth="1"/>
+    <col min="18" max="18" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -9027,7 +9048,7 @@
       </c>
       <c r="R1" s="20"/>
     </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>201</v>
       </c>
@@ -9078,7 +9099,7 @@
       </c>
       <c r="R2" s="18"/>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>201</v>
       </c>
@@ -9129,7 +9150,7 @@
       </c>
       <c r="R3" s="16"/>
     </row>
-    <row r="4" spans="2:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>201</v>
       </c>
@@ -9180,7 +9201,7 @@
       </c>
       <c r="R4" s="17"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>201</v>
       </c>
@@ -9231,7 +9252,7 @@
       </c>
       <c r="R5" s="16"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>201</v>
       </c>
@@ -9295,13 +9316,13 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.88671875" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -9321,7 +9342,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>258</v>
       </c>
@@ -9341,7 +9362,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>262</v>
       </c>
@@ -9372,12 +9393,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -9406,7 +9427,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>264</v>
       </c>
@@ -9446,12 +9467,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="34.7109375" customWidth="1"/>
+    <col min="7" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -9474,7 +9495,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>268</v>
       </c>
@@ -9497,7 +9518,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>272</v>
       </c>
@@ -9518,7 +9539,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>274</v>
       </c>
@@ -9550,14 +9571,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -9577,7 +9598,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>258</v>
       </c>
@@ -9597,7 +9618,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>262</v>
       </c>
@@ -9624,41 +9645,43 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC11"/>
+  <dimension ref="A1:BG11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BD1" sqref="BD1:DS1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="BC10" sqref="BC10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5546875" customWidth="1"/>
+    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="28.5703125" customWidth="1"/>
-    <col min="23" max="23" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="28.5546875" customWidth="1"/>
+    <col min="23" max="23" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
@@ -9824,8 +9847,20 @@
       <c r="BC1" s="45" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="2" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD1" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="2" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
         <v>538</v>
       </c>
@@ -9985,8 +10020,20 @@
         <v>545</v>
       </c>
       <c r="BC2" s="47"/>
-    </row>
-    <row r="3" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD2" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="BE2" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="BF2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="BG2" s="9" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="3" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>546</v>
       </c>
@@ -10144,8 +10191,20 @@
       </c>
       <c r="BB3" s="47"/>
       <c r="BC3" s="47"/>
-    </row>
-    <row r="4" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD3" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="BE3" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="BF3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="BG3" s="9" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="4" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>548</v>
       </c>
@@ -10303,8 +10362,20 @@
       </c>
       <c r="BB4" s="47"/>
       <c r="BC4" s="47"/>
-    </row>
-    <row r="5" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD4" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="BE4" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="BF4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="BG4" s="9" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="5" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>550</v>
       </c>
@@ -10464,8 +10535,20 @@
         <v>552</v>
       </c>
       <c r="BC5" s="47"/>
-    </row>
-    <row r="6" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD5" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="BE5" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="BF5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="BG5" s="9" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="6" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>553</v>
       </c>
@@ -10625,8 +10708,20 @@
         <v>545</v>
       </c>
       <c r="BC6" s="47"/>
-    </row>
-    <row r="7" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD6" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="BE6" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="BF6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="BG6" s="9" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="7" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>555</v>
       </c>
@@ -10786,8 +10881,20 @@
         <v>545</v>
       </c>
       <c r="BC7" s="47"/>
-    </row>
-    <row r="8" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD7" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="BE7" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="BF7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="BG7" s="9" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="8" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="47" t="s">
         <v>557</v>
       </c>
@@ -10947,8 +11054,20 @@
         <v>545</v>
       </c>
       <c r="BC8" s="47"/>
-    </row>
-    <row r="9" spans="1:55" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD8" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="BE8" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="BF8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="BG8" s="9" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="9" spans="1:59" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="47" t="s">
         <v>559</v>
       </c>
@@ -11106,8 +11225,20 @@
       </c>
       <c r="BB9" s="47"/>
       <c r="BC9" s="47"/>
-    </row>
-    <row r="10" spans="1:55" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD9" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="BE9" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="BF9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="BG9" s="9" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="10" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>561</v>
       </c>
@@ -11265,8 +11396,20 @@
       </c>
       <c r="BB10" s="47"/>
       <c r="BC10" s="47"/>
-    </row>
-    <row r="11" spans="1:55" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD10" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="BE10" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="BF10" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="BG10" s="9" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="11" spans="1:59" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
         <v>563</v>
       </c>
@@ -11426,6 +11569,18 @@
         <v>545</v>
       </c>
       <c r="BC11" s="47"/>
+      <c r="BD11" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="BE11" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="BF11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="BG11" s="9" t="s">
+        <v>586</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
added script for add loan type screen
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation/TestData/TestData.xlsx
+++ b/src/main/resources/config/automation/TestData/TestData.xlsx
@@ -24,12 +24,12 @@
     <sheet name="LoyaltyPlan" sheetId="16" r:id="rId15"/>
     <sheet name="Prepaid_Application_Upload" sheetId="17" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2395" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2450" uniqueCount="595">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1790,6 +1790,30 @@
   </si>
   <si>
     <t>Accounting, Auditing, and Bookkeeping Services [8931]</t>
+  </si>
+  <si>
+    <t>HolidayType</t>
+  </si>
+  <si>
+    <t>LoanType</t>
+  </si>
+  <si>
+    <t>DraftNeeded</t>
+  </si>
+  <si>
+    <t>LoanTypeCreditLimit</t>
+  </si>
+  <si>
+    <t>LoanTypeCashLimit</t>
+  </si>
+  <si>
+    <t>Holiday [H]</t>
+  </si>
+  <si>
+    <t>Loan below credit limit [LOANCR]</t>
+  </si>
+  <si>
+    <t>Retail Transaction to Loan [LOANPUR]</t>
   </si>
 </sst>
 </file>
@@ -9645,10 +9669,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BG11"/>
+  <dimension ref="A1:BL11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="BC10" sqref="BC10"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="BK3" sqref="BK3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9679,9 +9703,10 @@
     <col min="30" max="30" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="46" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
@@ -9859,8 +9884,23 @@
       <c r="BG1" s="1" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="2" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BH1" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="2" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
         <v>538</v>
       </c>
@@ -10032,8 +10072,23 @@
       <c r="BG2" s="9" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="3" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BH2" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="BI2" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="BJ2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BK2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BL2" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>546</v>
       </c>
@@ -10203,8 +10258,23 @@
       <c r="BG3" s="9" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="4" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BH3" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="BI3" s="9" t="s">
+        <v>594</v>
+      </c>
+      <c r="BJ3" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BK3" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BL3" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>548</v>
       </c>
@@ -10374,8 +10444,23 @@
       <c r="BG4" s="9" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="5" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BH4" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="BI4" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="BJ4" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BK4" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BL4" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>550</v>
       </c>
@@ -10547,8 +10632,23 @@
       <c r="BG5" s="9" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="6" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BH5" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="BI5" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="BJ5" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BK5" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BL5" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>553</v>
       </c>
@@ -10720,8 +10820,23 @@
       <c r="BG6" s="9" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="7" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BH6" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="BI6" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="BJ6" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BK6" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BL6" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>555</v>
       </c>
@@ -10893,8 +11008,23 @@
       <c r="BG7" s="9" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="8" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BH7" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="BI7" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="BJ7" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BK7" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BL7" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="47" t="s">
         <v>557</v>
       </c>
@@ -11066,8 +11196,23 @@
       <c r="BG8" s="9" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="9" spans="1:59" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BH8" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="BI8" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="BJ8" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BK8" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BL8" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:64" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="47" t="s">
         <v>559</v>
       </c>
@@ -11237,8 +11382,23 @@
       <c r="BG9" s="9" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="10" spans="1:59" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BH9" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="BI9" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="BJ9" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BK9" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BL9" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>561</v>
       </c>
@@ -11408,8 +11568,23 @@
       <c r="BG10" s="9" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="11" spans="1:59" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BH10" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="BI10" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="BJ10" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BK10" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BL10" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:64" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
         <v>563</v>
       </c>
@@ -11580,6 +11755,21 @@
       </c>
       <c r="BG11" s="9" t="s">
         <v>586</v>
+      </c>
+      <c r="BH11" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="BI11" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="BJ11" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BK11" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BL11" s="9" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
script changes for loan plan
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation/TestData/TestData.xlsx
+++ b/src/main/resources/config/automation/TestData/TestData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2450" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2472" uniqueCount="598">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1814,6 +1814,15 @@
   </si>
   <si>
     <t>Retail Transaction to Loan [LOANPUR]</t>
+  </si>
+  <si>
+    <t>ProgramWalletPromotion</t>
+  </si>
+  <si>
+    <t>DefaultLoanPlan</t>
+  </si>
+  <si>
+    <t>Program [0]</t>
   </si>
 </sst>
 </file>
@@ -9669,10 +9678,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL11"/>
+  <dimension ref="A1:BN11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
-      <selection activeCell="BK3" sqref="BK3"/>
+    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
+      <selection activeCell="BM1" sqref="BM1:BN11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9704,9 +9713,11 @@
     <col min="55" max="55" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="46" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
@@ -9899,8 +9910,14 @@
       <c r="BL1" s="1" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="2" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM1" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="2" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
         <v>538</v>
       </c>
@@ -10087,8 +10104,14 @@
       <c r="BL2" s="9" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="3" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM2" s="47" t="s">
+        <v>597</v>
+      </c>
+      <c r="BN2" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
         <v>546</v>
       </c>
@@ -10273,8 +10296,14 @@
       <c r="BL3" s="9" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="4" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM3" s="47" t="s">
+        <v>597</v>
+      </c>
+      <c r="BN3" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="47" t="s">
         <v>548</v>
       </c>
@@ -10459,8 +10488,14 @@
       <c r="BL4" s="9" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="5" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM4" s="47" t="s">
+        <v>597</v>
+      </c>
+      <c r="BN4" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>550</v>
       </c>
@@ -10647,8 +10682,14 @@
       <c r="BL5" s="9" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="6" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM5" s="47" t="s">
+        <v>597</v>
+      </c>
+      <c r="BN5" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="47" t="s">
         <v>553</v>
       </c>
@@ -10835,8 +10876,14 @@
       <c r="BL6" s="9" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="7" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM6" s="47" t="s">
+        <v>597</v>
+      </c>
+      <c r="BN6" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47" t="s">
         <v>555</v>
       </c>
@@ -11023,8 +11070,14 @@
       <c r="BL7" s="9" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="8" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM7" s="47" t="s">
+        <v>597</v>
+      </c>
+      <c r="BN7" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="47" t="s">
         <v>557</v>
       </c>
@@ -11211,8 +11264,14 @@
       <c r="BL8" s="9" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="9" spans="1:64" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM8" s="47" t="s">
+        <v>597</v>
+      </c>
+      <c r="BN8" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:66" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="47" t="s">
         <v>559</v>
       </c>
@@ -11397,8 +11456,14 @@
       <c r="BL9" s="9" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="10" spans="1:64" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM9" s="47" t="s">
+        <v>597</v>
+      </c>
+      <c r="BN9" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:66" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>561</v>
       </c>
@@ -11583,8 +11648,14 @@
       <c r="BL10" s="9" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="11" spans="1:64" s="50" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BM10" s="47" t="s">
+        <v>597</v>
+      </c>
+      <c r="BN10" s="47" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:66" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
         <v>563</v>
       </c>
@@ -11769,6 +11840,12 @@
         <v>230</v>
       </c>
       <c r="BL11" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BM11" s="47" t="s">
+        <v>597</v>
+      </c>
+      <c r="BN11" s="47" t="s">
         <v>230</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Channel Routing Plan Account range routing Linking API to Institution Aggregate Load Limits Alerts
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation/TestData/TestData.xlsx
+++ b/src/main/resources/config/automation/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="8970" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="8970" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="S181372" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2420" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2442" uniqueCount="615">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1817,6 +1817,63 @@
   </si>
   <si>
     <t>WIBMO [002]</t>
+  </si>
+  <si>
+    <t>AccountRangeFrom</t>
+  </si>
+  <si>
+    <t>AccountRangeTo</t>
+  </si>
+  <si>
+    <t>currencyCodeTxt</t>
+  </si>
+  <si>
+    <t>monthlyLimitTxt</t>
+  </si>
+  <si>
+    <t>monthlyVelocityTxt</t>
+  </si>
+  <si>
+    <t>yearlyLimitTxt</t>
+  </si>
+  <si>
+    <t>yearlyVelocityTxt</t>
+  </si>
+  <si>
+    <t>comparisonOperator</t>
+  </si>
+  <si>
+    <t>ruleCode</t>
+  </si>
+  <si>
+    <t>ruleValue</t>
+  </si>
+  <si>
+    <t>APILInkingUserID</t>
+  </si>
+  <si>
+    <t>525252523612345</t>
+  </si>
+  <si>
+    <t>525252523692345</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>100000000000000000000000</t>
+  </si>
+  <si>
+    <t>10000000000000000000</t>
+  </si>
+  <si>
+    <t>= [=]</t>
+  </si>
+  <si>
+    <t>Male</t>
   </si>
 </sst>
 </file>
@@ -5909,10 +5966,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DN177"/>
+  <dimension ref="A1:DY177"/>
   <sheetViews>
-    <sheetView topLeftCell="BH6" workbookViewId="0">
-      <selection activeCell="BR2" sqref="BR2:BR8"/>
+    <sheetView tabSelected="1" topLeftCell="CR1" workbookViewId="0">
+      <selection activeCell="DO1" sqref="DO1:DY2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5930,7 +5987,7 @@
     <col min="97" max="97" width="10.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:118" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:129" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -6283,8 +6340,41 @@
         <v>434</v>
       </c>
       <c r="DN1" s="4"/>
-    </row>
-    <row r="2" spans="1:118" ht="90" x14ac:dyDescent="0.25">
+      <c r="DO1" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="DP1" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="DQ1" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="DR1" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="DS1" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="DT1" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="DU1" s="4" t="s">
+        <v>602</v>
+      </c>
+      <c r="DV1" s="4" t="s">
+        <v>603</v>
+      </c>
+      <c r="DW1" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="DX1" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="DY1" s="4" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="2" spans="1:129" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>132</v>
       </c>
@@ -6610,8 +6700,41 @@
       <c r="DM2" s="9" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="3" spans="1:118" ht="90" x14ac:dyDescent="0.25">
+      <c r="DO2" s="9" t="s">
+        <v>607</v>
+      </c>
+      <c r="DP2" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="DQ2" s="9" t="s">
+        <v>609</v>
+      </c>
+      <c r="DR2" s="9" t="s">
+        <v>507</v>
+      </c>
+      <c r="DS2" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="DT2" s="9" t="s">
+        <v>611</v>
+      </c>
+      <c r="DU2" s="9" t="s">
+        <v>612</v>
+      </c>
+      <c r="DV2" s="49" t="s">
+        <v>613</v>
+      </c>
+      <c r="DW2" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="DX2" s="9" t="s">
+        <v>614</v>
+      </c>
+      <c r="DY2" s="9" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="3" spans="1:129" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>140</v>
       </c>
@@ -6890,7 +7013,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:118" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:129" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>150</v>
       </c>
@@ -7169,7 +7292,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:118" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:129" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>156</v>
       </c>
@@ -7448,7 +7571,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:118" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:129" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>163</v>
       </c>
@@ -7727,7 +7850,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:118" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:129" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>169</v>
       </c>
@@ -8008,7 +8131,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:118" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:129" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>175</v>
       </c>
@@ -8289,7 +8412,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:129" x14ac:dyDescent="0.25">
       <c r="CS9"/>
       <c r="CT9" t="s">
         <v>162</v>
@@ -8298,7 +8421,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:129" x14ac:dyDescent="0.25">
       <c r="CS10"/>
       <c r="CT10" t="s">
         <v>162</v>
@@ -8307,7 +8430,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:129" x14ac:dyDescent="0.25">
       <c r="CS11"/>
       <c r="CT11" t="s">
         <v>162</v>
@@ -8316,19 +8439,19 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:129" x14ac:dyDescent="0.25">
       <c r="CS12"/>
     </row>
-    <row r="13" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:129" x14ac:dyDescent="0.25">
       <c r="CS13"/>
     </row>
-    <row r="14" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:129" x14ac:dyDescent="0.25">
       <c r="CS14"/>
     </row>
-    <row r="15" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:129" x14ac:dyDescent="0.25">
       <c r="CS15"/>
     </row>
-    <row r="16" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:129" x14ac:dyDescent="0.25">
       <c r="CS16"/>
     </row>
     <row r="17" spans="97:97" x14ac:dyDescent="0.25">
@@ -9650,8 +9773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
data changes and story changes
</commit_message>
<xml_diff>
--- a/src/main/resources/config/automation/TestData/TestData.xlsx
+++ b/src/main/resources/config/automation/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="8970" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17265" windowHeight="4695" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="S181372" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="Prepaid_Application_Upload" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -10651,8 +10652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BS11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BF5" sqref="BF5"/>
+    <sheetView tabSelected="1" topLeftCell="BR1" workbookViewId="0">
+      <selection activeCell="BS2" sqref="BS2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10686,6 +10687,7 @@
     <col min="67" max="67" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="69" max="69" width="15" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:71" s="46" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>